<commit_message>
made glow function changed c0 c1 pins to 12 and  13
</commit_message>
<xml_diff>
--- a/led_cube.xlsx
+++ b/led_cube.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -65,6 +65,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +130,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -155,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -191,6 +200,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -497,11 +512,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +524,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -558,56 +573,56 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6">
-        <v>1</v>
-      </c>
-      <c r="O2" s="6">
-        <v>1</v>
-      </c>
-      <c r="P2" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14">
+        <v>0</v>
+      </c>
+      <c r="G2" s="14">
+        <v>0</v>
+      </c>
+      <c r="H2" s="14">
+        <v>0</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0</v>
+      </c>
+      <c r="J2" s="14">
+        <v>0</v>
+      </c>
+      <c r="K2" s="14">
+        <v>0</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14">
+        <v>1</v>
+      </c>
+      <c r="N2" s="14">
+        <v>1</v>
+      </c>
+      <c r="O2" s="14">
+        <v>1</v>
+      </c>
+      <c r="P2" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -626,7 +641,7 @@
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -675,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -724,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -773,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -822,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -871,7 +886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -920,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -969,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -988,7 +1003,7 @@
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>0</v>
       </c>
@@ -1036,8 +1051,12 @@
       <c r="Q12" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="1">
+        <v>14</v>
+      </c>
+      <c r="S12" s="13"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>0</v>
       </c>
@@ -1085,8 +1104,12 @@
       <c r="Q13" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="1">
+        <v>13</v>
+      </c>
+      <c r="S13" s="13"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>0</v>
       </c>
@@ -1134,8 +1157,12 @@
       <c r="Q14" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="1">
+        <v>13</v>
+      </c>
+      <c r="S14" s="13"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>0</v>
       </c>
@@ -1183,8 +1210,12 @@
       <c r="Q15" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15" s="1">
+        <v>11</v>
+      </c>
+      <c r="S15" s="13"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>0</v>
       </c>
@@ -1232,8 +1263,12 @@
       <c r="Q16" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="1">
+        <v>11</v>
+      </c>
+      <c r="S16" s="13"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>0</v>
       </c>
@@ -1281,8 +1316,12 @@
       <c r="Q17" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="1">
+        <v>7</v>
+      </c>
+      <c r="S17" s="13"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>0</v>
       </c>
@@ -1330,8 +1369,12 @@
       <c r="Q18" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="1">
+        <v>7</v>
+      </c>
+      <c r="S18" s="13"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1350,7 +1393,7 @@
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>0</v>
       </c>
@@ -1399,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>0</v>
       </c>
@@ -1448,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>0</v>
       </c>
@@ -1497,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>0</v>
       </c>
@@ -1546,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>0</v>
       </c>
@@ -1595,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>0</v>
       </c>
@@ -1644,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>0</v>
       </c>
@@ -1693,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H28" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed led_shapes to LED_8x8x8 added multiple tabs for easy coding
</commit_message>
<xml_diff>
--- a/led_cube.xlsx
+++ b/led_cube.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -69,7 +70,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +97,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -241,6 +248,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1784,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2042,6 +2058,14 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
@@ -2052,6 +2076,14 @@
       <c r="F11" s="16"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="16"/>
     </row>
     <row r="12" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
@@ -2062,6 +2094,14 @@
       <c r="F12" s="16"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="16"/>
     </row>
     <row r="13" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
@@ -2072,6 +2112,14 @@
       <c r="F13" s="16"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16"/>
     </row>
     <row r="14" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
@@ -2082,6 +2130,14 @@
       <c r="F14" s="16"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="16"/>
     </row>
     <row r="15" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
@@ -2092,6 +2148,14 @@
       <c r="F15" s="16"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="16"/>
     </row>
     <row r="16" spans="1:26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
@@ -2102,8 +2166,16 @@
       <c r="F16" s="16"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="16"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="16"/>
+    </row>
+    <row r="17" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -2112,6 +2184,366 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AB19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+    </row>
+    <row r="3" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="16">
+        <v>3</v>
+      </c>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="15"/>
+      <c r="AB3" s="15"/>
+    </row>
+    <row r="4" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>2</v>
+      </c>
+      <c r="F4" s="16">
+        <v>3</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16">
+        <v>2</v>
+      </c>
+      <c r="N4" s="15"/>
+      <c r="O4" s="16">
+        <v>4</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="16">
+        <v>7</v>
+      </c>
+      <c r="X4" s="16">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="16">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="15"/>
+    </row>
+    <row r="5" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16">
+        <v>8</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16">
+        <v>4</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16">
+        <v>1</v>
+      </c>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="16">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="16">
+        <v>8</v>
+      </c>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="16">
+        <v>4</v>
+      </c>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+    </row>
+    <row r="6" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16">
+        <v>7</v>
+      </c>
+      <c r="E6" s="16">
+        <v>6</v>
+      </c>
+      <c r="F6" s="16">
+        <v>5</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="16">
+        <v>8</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="16">
+        <v>6</v>
+      </c>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="16">
+        <v>1</v>
+      </c>
+      <c r="X6" s="16">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="16">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+    </row>
+    <row r="7" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="16">
+        <v>7</v>
+      </c>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+    </row>
+    <row r="8" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+    </row>
+    <row r="9" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+    </row>
+    <row r="12" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+    </row>
+    <row r="13" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+    </row>
+    <row r="14" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+    </row>
+    <row r="15" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+    </row>
+    <row r="16" spans="2:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+    </row>
+    <row r="17" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+    </row>
+    <row r="19" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>